<commit_message>
Dies Natalis HMJTI ke-5
</commit_message>
<xml_diff>
--- a/Administrasi/Surat Keluar Pengurus.xlsx
+++ b/Administrasi/Surat Keluar Pengurus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="555" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="555" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="98">
   <si>
     <t>Nomor Surat</t>
   </si>
@@ -255,6 +255,63 @@
   </si>
   <si>
     <t>Dekan FST</t>
+  </si>
+  <si>
+    <t>005/A2/HMJTI/SAINSTEK/X/2021</t>
+  </si>
+  <si>
+    <t>Paguyangan, 24 Oktober 2021</t>
+  </si>
+  <si>
+    <t>Paguyangan, 25 Oktober 2021</t>
+  </si>
+  <si>
+    <t>Dies Natalis HMJTI Ke-V</t>
+  </si>
+  <si>
+    <t>Sabtu, 30 Oktober 2021</t>
+  </si>
+  <si>
+    <t>Syukuran Dies Natalis Himpunan</t>
+  </si>
+  <si>
+    <t>005/A1/HMJTI/SAINSTEK/X/2021</t>
+  </si>
+  <si>
+    <t>BEM-FST</t>
+  </si>
+  <si>
+    <t>Kaprodi Informatika</t>
+  </si>
+  <si>
+    <t>Mahasiswa Informatika 2018</t>
+  </si>
+  <si>
+    <t>Mahasiswa Informatika 2019</t>
+  </si>
+  <si>
+    <t>Mahasiswa Informatika 2020</t>
+  </si>
+  <si>
+    <t>006/A1/HMJTI/SAINSTEK/X/2021</t>
+  </si>
+  <si>
+    <t>007/A1/HMJTI/SAINSTEK/X/2021</t>
+  </si>
+  <si>
+    <t>008/A1/HMJTI/SAINSTEK/X/2021</t>
+  </si>
+  <si>
+    <t>009/A1/HMJTI/SAINSTEK/X/2021</t>
+  </si>
+  <si>
+    <t>010/A1/HMJTI/SAINSTEK/X/2021</t>
+  </si>
+  <si>
+    <t>011/A1/HMJTI/SAINSTEK/X/2021</t>
+  </si>
+  <si>
+    <t>012/A1/HMJTI/SAINSTEK/X/2021</t>
   </si>
 </sst>
 </file>
@@ -302,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,6 +371,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,179 +678,467 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="35.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="6" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -801,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1006,6 +1354,43 @@
         <v>74</v>
       </c>
       <c r="M5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="3" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>